<commit_message>
Updates to AmazoniaBrazil conversion and non-raw template
</commit_message>
<xml_diff>
--- a/Load/ontology/ICEMR/amazonia/doc/AmazoniaBrazil_non-raw_detection_template.xlsx
+++ b/Load/ontology/ICEMR/amazonia/doc/AmazoniaBrazil_non-raw_detection_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/ICEMR/amazonia/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946A1330-DEBD-994E-8AA9-75716E6DF484}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5466E3-D663-9441-BE0D-F80683405B20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15720" yWindow="2240" windowWidth="25360" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_detection_template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>variable</t>
   </si>
@@ -140,12 +140,78 @@
   <si>
     <t>parasita</t>
   </si>
+  <si>
+    <t>pcrvefc</t>
+  </si>
+  <si>
+    <t>pcrve</t>
+  </si>
+  <si>
+    <t>pcrftvi</t>
+  </si>
+  <si>
+    <t>pcrftfc</t>
+  </si>
+  <si>
+    <t>pcrft</t>
+  </si>
+  <si>
+    <t>pcrveft</t>
+  </si>
+  <si>
+    <t>consens</t>
+  </si>
+  <si>
+    <t>pcrveftv</t>
+  </si>
+  <si>
+    <t>pcrveftf</t>
+  </si>
+  <si>
+    <t>gametoci</t>
+  </si>
+  <si>
+    <t>Plasmodium</t>
+  </si>
+  <si>
+    <t>qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium gametocytes</t>
+  </si>
+  <si>
+    <t>blood</t>
+  </si>
+  <si>
+    <t>Have to hack the label a little since this is for identification presence of gametocytes</t>
+  </si>
+  <si>
+    <t>Plasmodium falciparum (per uL)</t>
+  </si>
+  <si>
+    <t>microscopy and qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium species</t>
+  </si>
+  <si>
+    <t>FTA qPCR</t>
+  </si>
+  <si>
+    <t>venous blood qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium vivax (per uL)</t>
+  </si>
+  <si>
+    <t>Have to hack the label a little to include the units</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,13 +350,6 @@
       <strike/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -637,7 +696,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -646,7 +705,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1008,7 +1080,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,7 +1097,8 @@
     <col min="10" max="10" width="15.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="22.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="23.33203125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="30.33203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="30.33203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="30.33203125" style="2" customWidth="1"/>
     <col min="15" max="16" width="18.33203125" style="2" customWidth="1"/>
     <col min="17" max="17" width="17.1640625" style="3" customWidth="1"/>
     <col min="18" max="18" width="10.83203125" style="3"/>
@@ -1035,7 +1108,7 @@
     <col min="22" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1142,7 @@
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -1082,7 +1155,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="102" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1108,7 +1181,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1127,7 +1200,7 @@
       <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="2" t="str">
+      <c r="M3" s="4" t="str">
         <f>TRIM(IF($G3="",$F3,"")
 &amp;IF($G3&lt;&gt;"",$G3,"")
 &amp;IF($H3&lt;&gt;""," "&amp;$H3,"")
@@ -1150,7 +1223,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1169,8 +1242,8 @@
       <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="2" t="str">
-        <f t="shared" ref="M4:M13" si="0">TRIM(IF($G4="",$F4,"")
+      <c r="M4" s="4" t="str">
+        <f t="shared" ref="M4:M14" si="0">TRIM(IF($G4="",$F4,"")
 &amp;IF($G4&lt;&gt;"",$G4,"")
 &amp;IF($H4&lt;&gt;""," "&amp;$H4,"")
 &amp;IF(OR($H4="LT",$H4="ST",$H4&lt;&gt;""),"-pos","")
@@ -1181,65 +1254,441 @@
         <v>Parasite species, by microscopy</v>
       </c>
       <c r="N4" s="2" t="str">
-        <f t="shared" ref="N4:N13" si="1">TRIM($E4&amp;" in "&amp;$B4)</f>
+        <f t="shared" ref="N4:N14" si="1">TRIM($E4&amp;" in "&amp;$B4)</f>
         <v>Eukaryota in stool</v>
       </c>
       <c r="O4" s="2" t="str">
-        <f t="shared" ref="O4:O13" si="2">TRIM($D4&amp;" in "&amp;$B4)</f>
+        <f t="shared" ref="O4:O14" si="2">TRIM($D4&amp;" in "&amp;$B4)</f>
         <v>Eukaryota in stool</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
+    <row r="5" spans="1:21" s="7" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="M5" s="8" t="str">
+        <f>TRIM(IF($G5="",$F5,"")
+&amp;IF($G5&lt;&gt;"",$G5,"")
+&amp;IF($H5&lt;&gt;""," "&amp;$H5,"")
+&amp;IF(OR($H5="LT",$H5="ST",$H5&lt;&gt;""),"-pos","")
+&amp;IF($J5&lt;&gt;""," "&amp;$J5,"")
+&amp;IF($I5&lt;&gt;""," "&amp;$I5&amp;"-pos","")
+&amp;IF($K5&lt;&gt;""," "&amp;$K5&amp;"-neg","")
+&amp;", by "&amp;$C5)</f>
+        <v>Plasmodium species, by microscopy and qPCR</v>
+      </c>
+      <c r="N5" s="6" t="str">
+        <f>TRIM($E5&amp;" in "&amp;$B5)</f>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O5" s="6" t="str">
+        <f>TRIM($D5&amp;" in "&amp;$B5)</f>
+        <v>Eukaryota in blood</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="U5" s="6"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="G6"/>
-      <c r="H6"/>
+    <row r="6" spans="1:21" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="8" t="str">
+        <f>TRIM(IF($G6="",$F6,"")
+&amp;IF($G6&lt;&gt;"",$G6,"")
+&amp;IF($H6&lt;&gt;""," "&amp;$H6,"")
+&amp;IF(OR($H6="LT",$H6="ST",$H6&lt;&gt;""),"-pos","")
+&amp;IF($J6&lt;&gt;""," "&amp;$J6,"")
+&amp;IF($I6&lt;&gt;""," "&amp;$I6&amp;"-pos","")
+&amp;IF($K6&lt;&gt;""," "&amp;$K6&amp;"-neg","")
+&amp;", by "&amp;$C6)</f>
+        <v>Plasmodium gametocytes, by qPCR</v>
+      </c>
+      <c r="N6" s="6" t="str">
+        <f>TRIM($E6&amp;" in "&amp;$B6)</f>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O6" s="6" t="str">
+        <f>TRIM($D6&amp;" in "&amp;$B6)</f>
+        <v>Eukaryota in blood</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="U6" s="6"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-      <c r="F7"/>
+    <row r="7" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="G7"/>
       <c r="H7"/>
+      <c r="M7" s="4" t="str">
+        <f>TRIM(IF($G7="",$F7,"")
+&amp;IF($G7&lt;&gt;"",$G7,"")
+&amp;IF($H7&lt;&gt;""," "&amp;$H7,"")
+&amp;IF(OR($H7="LT",$H7="ST",$H7&lt;&gt;""),"-pos","")
+&amp;IF($J7&lt;&gt;""," "&amp;$J7,"")
+&amp;IF($I7&lt;&gt;""," "&amp;$I7&amp;"-pos","")
+&amp;IF($K7&lt;&gt;""," "&amp;$K7&amp;"-neg","")
+&amp;", by "&amp;$C7)</f>
+        <v>Plasmodium falciparum (per uL), by venous blood qPCR</v>
+      </c>
+      <c r="N7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O7" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Eukaryota in blood</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8"/>
-      <c r="F8"/>
+    <row r="8" spans="1:21" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="G8"/>
       <c r="H8"/>
+      <c r="M8" s="4" t="str">
+        <f>TRIM(IF($G8="",$F8,"")
+&amp;IF($G8&lt;&gt;"",$G8,"")
+&amp;IF($H8&lt;&gt;""," "&amp;$H8,"")
+&amp;IF(OR($H8="LT",$H8="ST",$H8&lt;&gt;""),"-pos","")
+&amp;IF($J8&lt;&gt;""," "&amp;$J8,"")
+&amp;IF($I8&lt;&gt;""," "&amp;$I8&amp;"-pos","")
+&amp;IF($K8&lt;&gt;""," "&amp;$K8&amp;"-neg","")
+&amp;", by "&amp;$C8)</f>
+        <v>Plasmodium falciparum (per uL), by FTA qPCR</v>
+      </c>
+      <c r="N8" s="2" t="str">
+        <f>TRIM($E8&amp;" in "&amp;$B8)</f>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O8" s="2" t="str">
+        <f>TRIM($D8&amp;" in "&amp;$B8)</f>
+        <v>Eukaryota in blood</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9"/>
-      <c r="G9"/>
-      <c r="H9"/>
+    <row r="9" spans="1:21" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="8" t="str">
+        <f>TRIM(IF($G9="",$F9,"")
+&amp;IF($G9&lt;&gt;"",$G9,"")
+&amp;IF($H9&lt;&gt;""," "&amp;$H9,"")
+&amp;IF(OR($H9="LT",$H9="ST",$H9&lt;&gt;""),"-pos","")
+&amp;IF($J9&lt;&gt;""," "&amp;$J9,"")
+&amp;IF($I9&lt;&gt;""," "&amp;$I9&amp;"-pos","")
+&amp;IF($K9&lt;&gt;""," "&amp;$K9&amp;"-neg","")
+&amp;", by "&amp;$C9)</f>
+        <v>Plasmodium falciparum (per uL), by qPCR</v>
+      </c>
+      <c r="N9" s="6" t="str">
+        <f>TRIM($E9&amp;" in "&amp;$B9)</f>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O9" s="6" t="str">
+        <f>TRIM($D9&amp;" in "&amp;$B9)</f>
+        <v>Eukaryota in blood</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="U9" s="6"/>
     </row>
-    <row r="10" spans="1:16" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10"/>
+    <row r="10" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="G10"/>
       <c r="H10"/>
+      <c r="M10" s="4" t="str">
+        <f>TRIM(IF($G10="",$F10,"")
+&amp;IF($G10&lt;&gt;"",$G10,"")
+&amp;IF($H10&lt;&gt;""," "&amp;$H10,"")
+&amp;IF(OR($H10="LT",$H10="ST",$H10&lt;&gt;""),"-pos","")
+&amp;IF($J10&lt;&gt;""," "&amp;$J10,"")
+&amp;IF($I10&lt;&gt;""," "&amp;$I10&amp;"-pos","")
+&amp;IF($K10&lt;&gt;""," "&amp;$K10&amp;"-neg","")
+&amp;", by "&amp;$C10)</f>
+        <v>Plasmodium vivax (per uL), by FTA qPCR</v>
+      </c>
+      <c r="N10" s="2" t="str">
+        <f>TRIM($E10&amp;" in "&amp;$B10)</f>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O10" s="2" t="str">
+        <f>TRIM($D10&amp;" in "&amp;$B10)</f>
+        <v>Eukaryota in blood</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
+    <row r="11" spans="1:21" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="M11" s="8" t="str">
+        <f>TRIM(IF($G11="",$F11,"")
+&amp;IF($G11&lt;&gt;"",$G11,"")
+&amp;IF($H11&lt;&gt;""," "&amp;$H11,"")
+&amp;IF(OR($H11="LT",$H11="ST",$H11&lt;&gt;""),"-pos","")
+&amp;IF($J11&lt;&gt;""," "&amp;$J11,"")
+&amp;IF($I11&lt;&gt;""," "&amp;$I11&amp;"-pos","")
+&amp;IF($K11&lt;&gt;""," "&amp;$K11&amp;"-neg","")
+&amp;", by "&amp;$C11)</f>
+        <v>Plasmodium vivax (per uL), by qPCR</v>
+      </c>
+      <c r="N11" s="6" t="str">
+        <f>TRIM($E11&amp;" in "&amp;$B11)</f>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O11" s="6" t="str">
+        <f>TRIM($D11&amp;" in "&amp;$B11)</f>
+        <v>Eukaryota in blood</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="U11" s="6"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12"/>
-      <c r="C12" s="4"/>
-      <c r="F12"/>
+    <row r="12" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="G12"/>
       <c r="H12"/>
+      <c r="M12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Plasmodium species, by venous blood qPCR</v>
+      </c>
+      <c r="N12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Eukaryota in blood</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13"/>
+    <row r="13" spans="1:21" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="M13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Plasmodium species, by FTA qPCR</v>
+      </c>
+      <c r="N13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O13" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Eukaryota in blood</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="7" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="M14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Plasmodium species, by qPCR</v>
+      </c>
+      <c r="N14" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Plasmodium in blood</v>
+      </c>
+      <c r="O14" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Eukaryota in blood</v>
+      </c>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="U14" s="6"/>
     </row>
     <row r="19" spans="17:17" x14ac:dyDescent="0.2">
       <c r="Q19" s="1"/>

</xml_diff>